<commit_message>
Excel Data imported to List
</commit_message>
<xml_diff>
--- a/src/main/resources/kynhood.xlsx
+++ b/src/main/resources/kynhood.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14540" windowHeight="5100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14540" windowHeight="2660"/>
   </bookViews>
   <sheets>
     <sheet name="klips_data" sheetId="1" r:id="rId1"/>
@@ -389,7 +389,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>